<commit_message>
Fix version suffix. Misc fixes.
</commit_message>
<xml_diff>
--- a/analyze_nhej/experiment_info.xlsx
+++ b/analyze_nhej/experiment_info.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="609" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="669" uniqueCount="191">
   <si>
     <t>cell_line</t>
   </si>
@@ -112,6 +112,15 @@
     <t>R2</t>
   </si>
   <si>
+    <t>merged</t>
+  </si>
+  <si>
+    <t>new</t>
+  </si>
+  <si>
+    <t>old</t>
+  </si>
+  <si>
     <t>['yjl296', 'yjl297', 'yjl298', 'yjl299']</t>
   </si>
   <si>
@@ -184,82 +193,82 @@
     <t>['yjl217', 'yjl218', 'yjl219', 'yjl220']</t>
   </si>
   <si>
+    <t>['yjl89_yjl349', 'yjl90_yjl350', 'yjl91_yjl351', 'yjl92_yjl352']</t>
+  </si>
+  <si>
+    <t>['yjl349', 'yjl350', 'yjl351', 'yjl352']</t>
+  </si>
+  <si>
     <t>['yjl89', 'yjl90', 'yjl91', 'yjl92']</t>
   </si>
   <si>
-    <t>['yjl349', 'yjl350', 'yjl351', 'yjl352']</t>
-  </si>
-  <si>
-    <t>['yjl89_yjl349', 'yjl90_yjl350', 'yjl91_yjl351', 'yjl92_yjl352']</t>
+    <t>['yjl93_yjl353', 'yjl94_yjl354', 'yjl95_yjl355', 'yjl96_yjl356']</t>
+  </si>
+  <si>
+    <t>['yjl353', 'yjl354', 'yjl355', 'yjl356']</t>
   </si>
   <si>
     <t>['yjl93', 'yjl94', 'yjl95', 'yjl96']</t>
   </si>
   <si>
-    <t>['yjl353', 'yjl354', 'yjl355', 'yjl356']</t>
-  </si>
-  <si>
-    <t>['yjl93_yjl353', 'yjl94_yjl354', 'yjl95_yjl355', 'yjl96_yjl356']</t>
-  </si>
-  <si>
-    <t>1DSB_R1_branch_1.fa</t>
-  </si>
-  <si>
-    <t>1DSB_R1_cmv_1.fa</t>
-  </si>
-  <si>
-    <t>1DSB_R1_sense_1.fa</t>
-  </si>
-  <si>
-    <t>1DSB_R2_branch_1.fa</t>
-  </si>
-  <si>
-    <t>1DSB_R2_cmv_1.fa</t>
-  </si>
-  <si>
-    <t>1DSB_R2_sense_1.fa</t>
-  </si>
-  <si>
-    <t>2DSB_R1_branch_1.fa</t>
-  </si>
-  <si>
-    <t>2DSB_R2_branch_1.fa</t>
-  </si>
-  <si>
-    <t>2DSB_R1_cmv_1.fa</t>
-  </si>
-  <si>
-    <t>2DSB_R2_cmv_1.fa</t>
-  </si>
-  <si>
-    <t>2DSB_R1_sense_1.fa</t>
-  </si>
-  <si>
-    <t>2DSB_R2_sense_1.fa</t>
-  </si>
-  <si>
-    <t>2DSBanti_R1_antisense_1.fa</t>
-  </si>
-  <si>
-    <t>2DSBanti_R1_antisense_2.fa</t>
-  </si>
-  <si>
-    <t>2DSBanti_R2_antisense_1.fa</t>
-  </si>
-  <si>
-    <t>2DSBanti_R2_antisense_2.fa</t>
-  </si>
-  <si>
-    <t>2DSBanti_R1_splicing_1.fa</t>
-  </si>
-  <si>
-    <t>2DSBanti_R1_splicing_2.fa</t>
-  </si>
-  <si>
-    <t>2DSBanti_R2_splicing_1.fa</t>
-  </si>
-  <si>
-    <t>2DSBanti_R2_splicing_2.fa</t>
+    <t>1DSB_R1_branch.fa</t>
+  </si>
+  <si>
+    <t>1DSB_R1_cmv.fa</t>
+  </si>
+  <si>
+    <t>1DSB_R1_sense.fa</t>
+  </si>
+  <si>
+    <t>1DSB_R2_branch.fa</t>
+  </si>
+  <si>
+    <t>1DSB_R2_cmv.fa</t>
+  </si>
+  <si>
+    <t>1DSB_R2_sense.fa</t>
+  </si>
+  <si>
+    <t>2DSB_R1_branch.fa</t>
+  </si>
+  <si>
+    <t>2DSB_R2_branch.fa</t>
+  </si>
+  <si>
+    <t>2DSB_R1_cmv.fa</t>
+  </si>
+  <si>
+    <t>2DSB_R2_cmv.fa</t>
+  </si>
+  <si>
+    <t>2DSB_R1_sense.fa</t>
+  </si>
+  <si>
+    <t>2DSB_R2_sense.fa</t>
+  </si>
+  <si>
+    <t>2DSBanti_R1_antisense_new.fa</t>
+  </si>
+  <si>
+    <t>2DSBanti_R1_antisense_old.fa</t>
+  </si>
+  <si>
+    <t>2DSBanti_R2_antisense_new.fa</t>
+  </si>
+  <si>
+    <t>2DSBanti_R2_antisense_old.fa</t>
+  </si>
+  <si>
+    <t>2DSBanti_R1_splicing_new.fa</t>
+  </si>
+  <si>
+    <t>2DSBanti_R1_splicing_old.fa</t>
+  </si>
+  <si>
+    <t>2DSBanti_R2_splicing_new.fa</t>
+  </si>
+  <si>
+    <t>2DSBanti_R2_splicing_old.fa</t>
   </si>
   <si>
     <t>[11021111, 11280773, 12426852, 11659042]</t>
@@ -370,214 +379,214 @@
     <t>[6177083, 6744517, 7507107, 7001340]</t>
   </si>
   <si>
+    <t>[14116151, 13475081, 13855904, 11992516]</t>
+  </si>
+  <si>
+    <t>[6302370, 5988345, 5741048, 5405939]</t>
+  </si>
+  <si>
     <t>[7813781, 7486736, 8114856, 6586577]</t>
   </si>
   <si>
-    <t>[6302370, 5988345, 5741048, 5405939]</t>
-  </si>
-  <si>
-    <t>[14116151, 13475081, 13855904, 11992516]</t>
+    <t>[13974893, 13342868, 13728439, 11868064]</t>
   </si>
   <si>
     <t>[6161112, 5856132, 5613583, 5281487]</t>
   </si>
   <si>
-    <t>[13974893, 13342868, 13728439, 11868064]</t>
+    <t>[13511783, 13789121, 12902873, 13400566]</t>
+  </si>
+  <si>
+    <t>[4177291, 4647120, 4405688, 5054324]</t>
   </si>
   <si>
     <t>[9334492, 9142001, 8497185, 8346242]</t>
   </si>
   <si>
-    <t>[4177291, 4647120, 4405688, 5054324]</t>
-  </si>
-  <si>
-    <t>[13511783, 13789121, 12902873, 13400566]</t>
+    <t>[13397050, 13677124, 12777909, 13272580]</t>
   </si>
   <si>
     <t>[4062558, 4535123, 4280724, 4926338]</t>
   </si>
   <si>
-    <t>[13397050, 13677124, 12777909, 13272580]</t>
-  </si>
-  <si>
-    <t>KO_sgA_R1_branch_30bpDown_1</t>
-  </si>
-  <si>
-    <t>KO_sgA_R1_cmv_30bpDown_1</t>
-  </si>
-  <si>
-    <t>KO_sgA_R1_sense_30bpDown_1</t>
-  </si>
-  <si>
-    <t>KO_sgB_R2_branch_30bpDown_1</t>
-  </si>
-  <si>
-    <t>KO_sgB_R2_cmv_30bpDown_1</t>
-  </si>
-  <si>
-    <t>KO_sgB_R2_sense_30bpDown_1</t>
-  </si>
-  <si>
-    <t>KO_sgA_R1_branch_noDSB_1</t>
-  </si>
-  <si>
-    <t>KO_sgA_R1_cmv_noDSB_1</t>
-  </si>
-  <si>
-    <t>KO_sgA_R1_sense_noDSB_1</t>
-  </si>
-  <si>
-    <t>KO_sgB_R2_branch_noDSB_1</t>
-  </si>
-  <si>
-    <t>KO_sgB_R2_cmv_noDSB_1</t>
-  </si>
-  <si>
-    <t>KO_sgB_R2_sense_noDSB_1</t>
-  </si>
-  <si>
-    <t>KO_sgA_R1_branch_1</t>
-  </si>
-  <si>
-    <t>KO_sgA_R1_cmv_1</t>
-  </si>
-  <si>
-    <t>KO_sgA_R1_sense_1</t>
-  </si>
-  <si>
-    <t>KO_sgB_R2_branch_1</t>
-  </si>
-  <si>
-    <t>KO_sgB_R2_cmv_1</t>
-  </si>
-  <si>
-    <t>KO_sgB_R2_sense_1</t>
-  </si>
-  <si>
-    <t>KO_sgAB_R1_branch_1</t>
-  </si>
-  <si>
-    <t>KO_sgAB_R2_branch_1</t>
-  </si>
-  <si>
-    <t>KO_sgAB_R1_cmv_1</t>
-  </si>
-  <si>
-    <t>KO_sgAB_R2_cmv_1</t>
-  </si>
-  <si>
-    <t>KO_sgAB_R1_sense_1</t>
-  </si>
-  <si>
-    <t>KO_sgAB_R2_sense_1</t>
-  </si>
-  <si>
-    <t>WT_sgA_R1_branch_30bpDown_1</t>
-  </si>
-  <si>
-    <t>WT_sgA_R1_cmv_30bpDown_1</t>
-  </si>
-  <si>
-    <t>WT_sgA_R1_sense_30bpDown_1</t>
-  </si>
-  <si>
-    <t>WT_sgB_R2_branch_30bpDown_1</t>
-  </si>
-  <si>
-    <t>WT_sgB_R2_cmv_30bpDown_1</t>
-  </si>
-  <si>
-    <t>WT_sgB_R2_sense_30bpDown_1</t>
-  </si>
-  <si>
-    <t>WT_sgA_R1_branch_noDSB_1</t>
-  </si>
-  <si>
-    <t>WT_sgA_R1_cmv_noDSB_1</t>
-  </si>
-  <si>
-    <t>WT_sgA_R1_sense_noDSB_1</t>
-  </si>
-  <si>
-    <t>WT_sgB_R2_branch_noDSB_1</t>
-  </si>
-  <si>
-    <t>WT_sgB_R2_cmv_noDSB_1</t>
-  </si>
-  <si>
-    <t>WT_sgB_R2_sense_noDSB_1</t>
-  </si>
-  <si>
-    <t>WT_sgA_R1_branch_1</t>
-  </si>
-  <si>
-    <t>WT_sgA_R1_cmv_1</t>
-  </si>
-  <si>
-    <t>WT_sgA_R1_sense_1</t>
-  </si>
-  <si>
-    <t>WT_sgB_R2_branch_1</t>
-  </si>
-  <si>
-    <t>WT_sgB_R2_cmv_1</t>
-  </si>
-  <si>
-    <t>WT_sgB_R2_sense_1</t>
-  </si>
-  <si>
-    <t>WT_sgAB_R1_branch_1</t>
-  </si>
-  <si>
-    <t>WT_sgAB_R2_branch_1</t>
-  </si>
-  <si>
-    <t>WT_sgAB_R1_cmv_1</t>
-  </si>
-  <si>
-    <t>WT_sgAB_R2_cmv_1</t>
-  </si>
-  <si>
-    <t>WT_sgAB_R1_sense_1</t>
-  </si>
-  <si>
-    <t>WT_sgAB_R2_sense_1</t>
-  </si>
-  <si>
-    <t>WT_sgCD_R1_antisense_1</t>
-  </si>
-  <si>
-    <t>WT_sgCD_R1_antisense_2</t>
-  </si>
-  <si>
-    <t>WT_sgCD_R1_antisense_3</t>
-  </si>
-  <si>
-    <t>WT_sgCD_R2_antisense_1</t>
-  </si>
-  <si>
-    <t>WT_sgCD_R2_antisense_2</t>
-  </si>
-  <si>
-    <t>WT_sgCD_R2_antisense_3</t>
-  </si>
-  <si>
-    <t>WT_sgCD_R1_splicing_1</t>
-  </si>
-  <si>
-    <t>WT_sgCD_R1_splicing_2</t>
-  </si>
-  <si>
-    <t>WT_sgCD_R1_splicing_3</t>
-  </si>
-  <si>
-    <t>WT_sgCD_R2_splicing_1</t>
-  </si>
-  <si>
-    <t>WT_sgCD_R2_splicing_2</t>
-  </si>
-  <si>
-    <t>WT_sgCD_R2_splicing_3</t>
+    <t>KO_sgA_R1_branch_30bpDown</t>
+  </si>
+  <si>
+    <t>KO_sgA_R1_cmv_30bpDown</t>
+  </si>
+  <si>
+    <t>KO_sgA_R1_sense_30bpDown</t>
+  </si>
+  <si>
+    <t>KO_sgB_R2_branch_30bpDown</t>
+  </si>
+  <si>
+    <t>KO_sgB_R2_cmv_30bpDown</t>
+  </si>
+  <si>
+    <t>KO_sgB_R2_sense_30bpDown</t>
+  </si>
+  <si>
+    <t>KO_sgA_R1_branch_noDSB</t>
+  </si>
+  <si>
+    <t>KO_sgA_R1_cmv_noDSB</t>
+  </si>
+  <si>
+    <t>KO_sgA_R1_sense_noDSB</t>
+  </si>
+  <si>
+    <t>KO_sgB_R2_branch_noDSB</t>
+  </si>
+  <si>
+    <t>KO_sgB_R2_cmv_noDSB</t>
+  </si>
+  <si>
+    <t>KO_sgB_R2_sense_noDSB</t>
+  </si>
+  <si>
+    <t>KO_sgA_R1_branch</t>
+  </si>
+  <si>
+    <t>KO_sgA_R1_cmv</t>
+  </si>
+  <si>
+    <t>KO_sgA_R1_sense</t>
+  </si>
+  <si>
+    <t>KO_sgB_R2_branch</t>
+  </si>
+  <si>
+    <t>KO_sgB_R2_cmv</t>
+  </si>
+  <si>
+    <t>KO_sgB_R2_sense</t>
+  </si>
+  <si>
+    <t>KO_sgAB_R1_branch</t>
+  </si>
+  <si>
+    <t>KO_sgAB_R2_branch</t>
+  </si>
+  <si>
+    <t>KO_sgAB_R1_cmv</t>
+  </si>
+  <si>
+    <t>KO_sgAB_R2_cmv</t>
+  </si>
+  <si>
+    <t>KO_sgAB_R1_sense</t>
+  </si>
+  <si>
+    <t>KO_sgAB_R2_sense</t>
+  </si>
+  <si>
+    <t>WT_sgA_R1_branch_30bpDown</t>
+  </si>
+  <si>
+    <t>WT_sgA_R1_cmv_30bpDown</t>
+  </si>
+  <si>
+    <t>WT_sgA_R1_sense_30bpDown</t>
+  </si>
+  <si>
+    <t>WT_sgB_R2_branch_30bpDown</t>
+  </si>
+  <si>
+    <t>WT_sgB_R2_cmv_30bpDown</t>
+  </si>
+  <si>
+    <t>WT_sgB_R2_sense_30bpDown</t>
+  </si>
+  <si>
+    <t>WT_sgA_R1_branch_noDSB</t>
+  </si>
+  <si>
+    <t>WT_sgA_R1_cmv_noDSB</t>
+  </si>
+  <si>
+    <t>WT_sgA_R1_sense_noDSB</t>
+  </si>
+  <si>
+    <t>WT_sgB_R2_branch_noDSB</t>
+  </si>
+  <si>
+    <t>WT_sgB_R2_cmv_noDSB</t>
+  </si>
+  <si>
+    <t>WT_sgB_R2_sense_noDSB</t>
+  </si>
+  <si>
+    <t>WT_sgA_R1_branch</t>
+  </si>
+  <si>
+    <t>WT_sgA_R1_cmv</t>
+  </si>
+  <si>
+    <t>WT_sgA_R1_sense</t>
+  </si>
+  <si>
+    <t>WT_sgB_R2_branch</t>
+  </si>
+  <si>
+    <t>WT_sgB_R2_cmv</t>
+  </si>
+  <si>
+    <t>WT_sgB_R2_sense</t>
+  </si>
+  <si>
+    <t>WT_sgAB_R1_branch</t>
+  </si>
+  <si>
+    <t>WT_sgAB_R2_branch</t>
+  </si>
+  <si>
+    <t>WT_sgAB_R1_cmv</t>
+  </si>
+  <si>
+    <t>WT_sgAB_R2_cmv</t>
+  </si>
+  <si>
+    <t>WT_sgAB_R1_sense</t>
+  </si>
+  <si>
+    <t>WT_sgAB_R2_sense</t>
+  </si>
+  <si>
+    <t>WT_sgCD_R1_antisense_merged</t>
+  </si>
+  <si>
+    <t>WT_sgCD_R1_antisense_new</t>
+  </si>
+  <si>
+    <t>WT_sgCD_R1_antisense_old</t>
+  </si>
+  <si>
+    <t>WT_sgCD_R2_antisense_merged</t>
+  </si>
+  <si>
+    <t>WT_sgCD_R2_antisense_new</t>
+  </si>
+  <si>
+    <t>WT_sgCD_R2_antisense_old</t>
+  </si>
+  <si>
+    <t>WT_sgCD_R1_splicing_merged</t>
+  </si>
+  <si>
+    <t>WT_sgCD_R1_splicing_new</t>
+  </si>
+  <si>
+    <t>WT_sgCD_R1_splicing_old</t>
+  </si>
+  <si>
+    <t>WT_sgCD_R2_splicing_merged</t>
+  </si>
+  <si>
+    <t>WT_sgCD_R2_splicing_new</t>
+  </si>
+  <si>
+    <t>WT_sgCD_R2_splicing_old</t>
   </si>
 </sst>
 </file>
@@ -1004,26 +1013,26 @@
       <c r="G2" t="s">
         <v>30</v>
       </c>
-      <c r="H2">
-        <v>1</v>
+      <c r="H2" t="s">
+        <v>17</v>
       </c>
       <c r="I2" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="J2">
         <v>97</v>
       </c>
       <c r="K2" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="L2" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="M2">
         <v>130</v>
       </c>
       <c r="N2" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -1048,26 +1057,26 @@
       <c r="G3" t="s">
         <v>30</v>
       </c>
-      <c r="H3">
-        <v>1</v>
+      <c r="H3" t="s">
+        <v>17</v>
       </c>
       <c r="I3" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="J3">
         <v>97</v>
       </c>
       <c r="K3" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="L3" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="M3">
         <v>130</v>
       </c>
       <c r="N3" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
     </row>
     <row r="4" spans="1:14">
@@ -1092,26 +1101,26 @@
       <c r="G4" t="s">
         <v>30</v>
       </c>
-      <c r="H4">
-        <v>1</v>
+      <c r="H4" t="s">
+        <v>17</v>
       </c>
       <c r="I4" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="J4">
         <v>97</v>
       </c>
       <c r="K4" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="L4" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="M4">
         <v>130</v>
       </c>
       <c r="N4" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
     </row>
     <row r="5" spans="1:14">
@@ -1136,26 +1145,26 @@
       <c r="G5" t="s">
         <v>31</v>
       </c>
-      <c r="H5">
-        <v>1</v>
+      <c r="H5" t="s">
+        <v>17</v>
       </c>
       <c r="I5" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="J5">
         <v>76</v>
       </c>
       <c r="K5" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="L5" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="M5">
         <v>130</v>
       </c>
       <c r="N5" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="6" spans="1:14">
@@ -1180,26 +1189,26 @@
       <c r="G6" t="s">
         <v>31</v>
       </c>
-      <c r="H6">
-        <v>1</v>
+      <c r="H6" t="s">
+        <v>17</v>
       </c>
       <c r="I6" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="J6">
         <v>76</v>
       </c>
       <c r="K6" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="L6" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="M6">
         <v>130</v>
       </c>
       <c r="N6" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
     </row>
     <row r="7" spans="1:14">
@@ -1224,26 +1233,26 @@
       <c r="G7" t="s">
         <v>31</v>
       </c>
-      <c r="H7">
-        <v>1</v>
+      <c r="H7" t="s">
+        <v>17</v>
       </c>
       <c r="I7" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="J7">
         <v>76</v>
       </c>
       <c r="K7" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="L7" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="M7">
         <v>130</v>
       </c>
       <c r="N7" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
     </row>
     <row r="8" spans="1:14">
@@ -1268,26 +1277,26 @@
       <c r="G8" t="s">
         <v>30</v>
       </c>
-      <c r="H8">
-        <v>1</v>
+      <c r="H8" t="s">
+        <v>17</v>
       </c>
       <c r="I8" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="J8">
         <v>67</v>
       </c>
       <c r="K8" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="L8" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="M8">
         <v>130</v>
       </c>
       <c r="N8" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
     </row>
     <row r="9" spans="1:14">
@@ -1312,26 +1321,26 @@
       <c r="G9" t="s">
         <v>30</v>
       </c>
-      <c r="H9">
-        <v>1</v>
+      <c r="H9" t="s">
+        <v>17</v>
       </c>
       <c r="I9" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="J9">
         <v>67</v>
       </c>
       <c r="K9" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="L9" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="M9">
         <v>130</v>
       </c>
       <c r="N9" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
     </row>
     <row r="10" spans="1:14">
@@ -1356,26 +1365,26 @@
       <c r="G10" t="s">
         <v>30</v>
       </c>
-      <c r="H10">
-        <v>1</v>
+      <c r="H10" t="s">
+        <v>17</v>
       </c>
       <c r="I10" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="J10">
         <v>67</v>
       </c>
       <c r="K10" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="L10" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="M10">
         <v>130</v>
       </c>
       <c r="N10" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="11" spans="1:14">
@@ -1400,26 +1409,26 @@
       <c r="G11" t="s">
         <v>31</v>
       </c>
-      <c r="H11">
-        <v>1</v>
+      <c r="H11" t="s">
+        <v>17</v>
       </c>
       <c r="I11" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="J11">
         <v>46</v>
       </c>
       <c r="K11" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="L11" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="M11">
         <v>130</v>
       </c>
       <c r="N11" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
     </row>
     <row r="12" spans="1:14">
@@ -1444,26 +1453,26 @@
       <c r="G12" t="s">
         <v>31</v>
       </c>
-      <c r="H12">
-        <v>1</v>
+      <c r="H12" t="s">
+        <v>17</v>
       </c>
       <c r="I12" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="J12">
         <v>46</v>
       </c>
       <c r="K12" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="L12" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="M12">
         <v>130</v>
       </c>
       <c r="N12" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
     </row>
     <row r="13" spans="1:14">
@@ -1488,26 +1497,26 @@
       <c r="G13" t="s">
         <v>31</v>
       </c>
-      <c r="H13">
-        <v>1</v>
+      <c r="H13" t="s">
+        <v>17</v>
       </c>
       <c r="I13" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="J13">
         <v>46</v>
       </c>
       <c r="K13" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="L13" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="M13">
         <v>130</v>
       </c>
       <c r="N13" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
     </row>
     <row r="14" spans="1:14">
@@ -1532,26 +1541,26 @@
       <c r="G14" t="s">
         <v>30</v>
       </c>
-      <c r="H14">
-        <v>1</v>
+      <c r="H14" t="s">
+        <v>17</v>
       </c>
       <c r="I14" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="J14">
         <v>67</v>
       </c>
       <c r="K14" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="L14" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="M14">
         <v>130</v>
       </c>
       <c r="N14" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
     </row>
     <row r="15" spans="1:14">
@@ -1576,26 +1585,26 @@
       <c r="G15" t="s">
         <v>30</v>
       </c>
-      <c r="H15">
-        <v>1</v>
+      <c r="H15" t="s">
+        <v>17</v>
       </c>
       <c r="I15" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="J15">
         <v>67</v>
       </c>
       <c r="K15" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="L15" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="M15">
         <v>130</v>
       </c>
       <c r="N15" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
     </row>
     <row r="16" spans="1:14">
@@ -1620,26 +1629,26 @@
       <c r="G16" t="s">
         <v>30</v>
       </c>
-      <c r="H16">
-        <v>1</v>
+      <c r="H16" t="s">
+        <v>17</v>
       </c>
       <c r="I16" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="J16">
         <v>67</v>
       </c>
       <c r="K16" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="L16" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="M16">
         <v>130</v>
       </c>
       <c r="N16" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
     </row>
     <row r="17" spans="1:14">
@@ -1664,26 +1673,26 @@
       <c r="G17" t="s">
         <v>31</v>
       </c>
-      <c r="H17">
-        <v>1</v>
+      <c r="H17" t="s">
+        <v>17</v>
       </c>
       <c r="I17" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="J17">
         <v>46</v>
       </c>
       <c r="K17" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="L17" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="M17">
         <v>130</v>
       </c>
       <c r="N17" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
     </row>
     <row r="18" spans="1:14">
@@ -1708,26 +1717,26 @@
       <c r="G18" t="s">
         <v>31</v>
       </c>
-      <c r="H18">
-        <v>1</v>
+      <c r="H18" t="s">
+        <v>17</v>
       </c>
       <c r="I18" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="J18">
         <v>46</v>
       </c>
       <c r="K18" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="L18" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="M18">
         <v>130</v>
       </c>
       <c r="N18" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
     </row>
     <row r="19" spans="1:14">
@@ -1752,26 +1761,26 @@
       <c r="G19" t="s">
         <v>31</v>
       </c>
-      <c r="H19">
-        <v>1</v>
+      <c r="H19" t="s">
+        <v>17</v>
       </c>
       <c r="I19" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="J19">
         <v>46</v>
       </c>
       <c r="K19" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="L19" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="M19">
         <v>130</v>
       </c>
       <c r="N19" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
     </row>
     <row r="20" spans="1:14">
@@ -1796,26 +1805,26 @@
       <c r="G20" t="s">
         <v>30</v>
       </c>
-      <c r="H20">
-        <v>1</v>
+      <c r="H20" t="s">
+        <v>17</v>
       </c>
       <c r="I20" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="J20">
         <v>67</v>
       </c>
       <c r="K20" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="L20" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="M20">
         <v>50</v>
       </c>
       <c r="N20" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
     </row>
     <row r="21" spans="1:14">
@@ -1840,26 +1849,26 @@
       <c r="G21" t="s">
         <v>31</v>
       </c>
-      <c r="H21">
-        <v>1</v>
+      <c r="H21" t="s">
+        <v>17</v>
       </c>
       <c r="I21" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="J21">
         <v>46</v>
       </c>
       <c r="K21" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="L21" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="M21">
         <v>50</v>
       </c>
       <c r="N21" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
     </row>
     <row r="22" spans="1:14">
@@ -1884,26 +1893,26 @@
       <c r="G22" t="s">
         <v>30</v>
       </c>
-      <c r="H22">
-        <v>1</v>
+      <c r="H22" t="s">
+        <v>17</v>
       </c>
       <c r="I22" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="J22">
         <v>67</v>
       </c>
       <c r="K22" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="L22" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="M22">
         <v>50</v>
       </c>
       <c r="N22" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
     </row>
     <row r="23" spans="1:14">
@@ -1928,26 +1937,26 @@
       <c r="G23" t="s">
         <v>31</v>
       </c>
-      <c r="H23">
-        <v>1</v>
+      <c r="H23" t="s">
+        <v>17</v>
       </c>
       <c r="I23" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="J23">
         <v>46</v>
       </c>
       <c r="K23" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="L23" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="M23">
         <v>50</v>
       </c>
       <c r="N23" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
     </row>
     <row r="24" spans="1:14">
@@ -1972,26 +1981,26 @@
       <c r="G24" t="s">
         <v>30</v>
       </c>
-      <c r="H24">
-        <v>1</v>
+      <c r="H24" t="s">
+        <v>17</v>
       </c>
       <c r="I24" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="J24">
         <v>67</v>
       </c>
       <c r="K24" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="L24" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="M24">
         <v>50</v>
       </c>
       <c r="N24" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
     </row>
     <row r="25" spans="1:14">
@@ -2016,26 +2025,26 @@
       <c r="G25" t="s">
         <v>31</v>
       </c>
-      <c r="H25">
-        <v>1</v>
+      <c r="H25" t="s">
+        <v>17</v>
       </c>
       <c r="I25" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="J25">
         <v>46</v>
       </c>
       <c r="K25" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="L25" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="M25">
         <v>50</v>
       </c>
       <c r="N25" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
     </row>
     <row r="26" spans="1:14">
@@ -2060,26 +2069,26 @@
       <c r="G26" t="s">
         <v>30</v>
       </c>
-      <c r="H26">
-        <v>1</v>
+      <c r="H26" t="s">
+        <v>17</v>
       </c>
       <c r="I26" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="J26">
         <v>97</v>
       </c>
       <c r="K26" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="L26" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="M26">
         <v>130</v>
       </c>
       <c r="N26" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
     </row>
     <row r="27" spans="1:14">
@@ -2104,26 +2113,26 @@
       <c r="G27" t="s">
         <v>30</v>
       </c>
-      <c r="H27">
-        <v>1</v>
+      <c r="H27" t="s">
+        <v>17</v>
       </c>
       <c r="I27" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="J27">
         <v>97</v>
       </c>
       <c r="K27" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="L27" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="M27">
         <v>130</v>
       </c>
       <c r="N27" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
     </row>
     <row r="28" spans="1:14">
@@ -2148,26 +2157,26 @@
       <c r="G28" t="s">
         <v>30</v>
       </c>
-      <c r="H28">
-        <v>1</v>
+      <c r="H28" t="s">
+        <v>17</v>
       </c>
       <c r="I28" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="J28">
         <v>97</v>
       </c>
       <c r="K28" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="L28" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="M28">
         <v>130</v>
       </c>
       <c r="N28" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
     </row>
     <row r="29" spans="1:14">
@@ -2192,26 +2201,26 @@
       <c r="G29" t="s">
         <v>31</v>
       </c>
-      <c r="H29">
-        <v>1</v>
+      <c r="H29" t="s">
+        <v>17</v>
       </c>
       <c r="I29" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="J29">
         <v>76</v>
       </c>
       <c r="K29" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="L29" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="M29">
         <v>130</v>
       </c>
       <c r="N29" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
     </row>
     <row r="30" spans="1:14">
@@ -2236,26 +2245,26 @@
       <c r="G30" t="s">
         <v>31</v>
       </c>
-      <c r="H30">
-        <v>1</v>
+      <c r="H30" t="s">
+        <v>17</v>
       </c>
       <c r="I30" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="J30">
         <v>76</v>
       </c>
       <c r="K30" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="L30" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="M30">
         <v>130</v>
       </c>
       <c r="N30" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
     </row>
     <row r="31" spans="1:14">
@@ -2280,26 +2289,26 @@
       <c r="G31" t="s">
         <v>31</v>
       </c>
-      <c r="H31">
-        <v>1</v>
+      <c r="H31" t="s">
+        <v>17</v>
       </c>
       <c r="I31" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="J31">
         <v>76</v>
       </c>
       <c r="K31" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="L31" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="M31">
         <v>130</v>
       </c>
       <c r="N31" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
     </row>
     <row r="32" spans="1:14">
@@ -2324,26 +2333,26 @@
       <c r="G32" t="s">
         <v>30</v>
       </c>
-      <c r="H32">
-        <v>1</v>
+      <c r="H32" t="s">
+        <v>17</v>
       </c>
       <c r="I32" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="J32">
         <v>67</v>
       </c>
       <c r="K32" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="L32" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="M32">
         <v>130</v>
       </c>
       <c r="N32" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
     </row>
     <row r="33" spans="1:14">
@@ -2368,26 +2377,26 @@
       <c r="G33" t="s">
         <v>30</v>
       </c>
-      <c r="H33">
-        <v>1</v>
+      <c r="H33" t="s">
+        <v>17</v>
       </c>
       <c r="I33" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="J33">
         <v>67</v>
       </c>
       <c r="K33" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="L33" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="M33">
         <v>130</v>
       </c>
       <c r="N33" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
     </row>
     <row r="34" spans="1:14">
@@ -2412,26 +2421,26 @@
       <c r="G34" t="s">
         <v>30</v>
       </c>
-      <c r="H34">
-        <v>1</v>
+      <c r="H34" t="s">
+        <v>17</v>
       </c>
       <c r="I34" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="J34">
         <v>67</v>
       </c>
       <c r="K34" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="L34" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="M34">
         <v>130</v>
       </c>
       <c r="N34" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
     </row>
     <row r="35" spans="1:14">
@@ -2456,26 +2465,26 @@
       <c r="G35" t="s">
         <v>31</v>
       </c>
-      <c r="H35">
-        <v>1</v>
+      <c r="H35" t="s">
+        <v>17</v>
       </c>
       <c r="I35" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="J35">
         <v>46</v>
       </c>
       <c r="K35" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="L35" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="M35">
         <v>130</v>
       </c>
       <c r="N35" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
     </row>
     <row r="36" spans="1:14">
@@ -2500,26 +2509,26 @@
       <c r="G36" t="s">
         <v>31</v>
       </c>
-      <c r="H36">
-        <v>1</v>
+      <c r="H36" t="s">
+        <v>17</v>
       </c>
       <c r="I36" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="J36">
         <v>46</v>
       </c>
       <c r="K36" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="L36" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="M36">
         <v>130</v>
       </c>
       <c r="N36" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
     </row>
     <row r="37" spans="1:14">
@@ -2544,26 +2553,26 @@
       <c r="G37" t="s">
         <v>31</v>
       </c>
-      <c r="H37">
-        <v>1</v>
+      <c r="H37" t="s">
+        <v>17</v>
       </c>
       <c r="I37" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="J37">
         <v>46</v>
       </c>
       <c r="K37" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="L37" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="M37">
         <v>130</v>
       </c>
       <c r="N37" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
     </row>
     <row r="38" spans="1:14">
@@ -2588,26 +2597,26 @@
       <c r="G38" t="s">
         <v>30</v>
       </c>
-      <c r="H38">
-        <v>1</v>
+      <c r="H38" t="s">
+        <v>17</v>
       </c>
       <c r="I38" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="J38">
         <v>67</v>
       </c>
       <c r="K38" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="L38" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="M38">
         <v>130</v>
       </c>
       <c r="N38" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
     </row>
     <row r="39" spans="1:14">
@@ -2632,26 +2641,26 @@
       <c r="G39" t="s">
         <v>30</v>
       </c>
-      <c r="H39">
-        <v>1</v>
+      <c r="H39" t="s">
+        <v>17</v>
       </c>
       <c r="I39" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="J39">
         <v>67</v>
       </c>
       <c r="K39" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="L39" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="M39">
         <v>130</v>
       </c>
       <c r="N39" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
     </row>
     <row r="40" spans="1:14">
@@ -2676,26 +2685,26 @@
       <c r="G40" t="s">
         <v>30</v>
       </c>
-      <c r="H40">
-        <v>1</v>
+      <c r="H40" t="s">
+        <v>17</v>
       </c>
       <c r="I40" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="J40">
         <v>67</v>
       </c>
       <c r="K40" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="L40" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="M40">
         <v>130</v>
       </c>
       <c r="N40" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
     </row>
     <row r="41" spans="1:14">
@@ -2720,26 +2729,26 @@
       <c r="G41" t="s">
         <v>31</v>
       </c>
-      <c r="H41">
-        <v>1</v>
+      <c r="H41" t="s">
+        <v>17</v>
       </c>
       <c r="I41" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="J41">
         <v>46</v>
       </c>
       <c r="K41" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="L41" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="M41">
         <v>130</v>
       </c>
       <c r="N41" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
     </row>
     <row r="42" spans="1:14">
@@ -2764,26 +2773,26 @@
       <c r="G42" t="s">
         <v>31</v>
       </c>
-      <c r="H42">
-        <v>1</v>
+      <c r="H42" t="s">
+        <v>17</v>
       </c>
       <c r="I42" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="J42">
         <v>46</v>
       </c>
       <c r="K42" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="L42" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="M42">
         <v>130</v>
       </c>
       <c r="N42" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
     </row>
     <row r="43" spans="1:14">
@@ -2808,26 +2817,26 @@
       <c r="G43" t="s">
         <v>31</v>
       </c>
-      <c r="H43">
-        <v>1</v>
+      <c r="H43" t="s">
+        <v>17</v>
       </c>
       <c r="I43" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="J43">
         <v>46</v>
       </c>
       <c r="K43" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="L43" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="M43">
         <v>130</v>
       </c>
       <c r="N43" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
     </row>
     <row r="44" spans="1:14">
@@ -2852,26 +2861,26 @@
       <c r="G44" t="s">
         <v>30</v>
       </c>
-      <c r="H44">
-        <v>1</v>
+      <c r="H44" t="s">
+        <v>17</v>
       </c>
       <c r="I44" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="J44">
         <v>67</v>
       </c>
       <c r="K44" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="L44" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="M44">
         <v>50</v>
       </c>
       <c r="N44" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
     </row>
     <row r="45" spans="1:14">
@@ -2896,26 +2905,26 @@
       <c r="G45" t="s">
         <v>31</v>
       </c>
-      <c r="H45">
-        <v>1</v>
+      <c r="H45" t="s">
+        <v>17</v>
       </c>
       <c r="I45" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="J45">
         <v>46</v>
       </c>
       <c r="K45" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="L45" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="M45">
         <v>50</v>
       </c>
       <c r="N45" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
     </row>
     <row r="46" spans="1:14">
@@ -2940,26 +2949,26 @@
       <c r="G46" t="s">
         <v>30</v>
       </c>
-      <c r="H46">
-        <v>1</v>
+      <c r="H46" t="s">
+        <v>17</v>
       </c>
       <c r="I46" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="J46">
         <v>67</v>
       </c>
       <c r="K46" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="L46" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="M46">
         <v>50</v>
       </c>
       <c r="N46" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
     </row>
     <row r="47" spans="1:14">
@@ -2984,26 +2993,26 @@
       <c r="G47" t="s">
         <v>31</v>
       </c>
-      <c r="H47">
-        <v>1</v>
+      <c r="H47" t="s">
+        <v>17</v>
       </c>
       <c r="I47" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="J47">
         <v>46</v>
       </c>
       <c r="K47" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="L47" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="M47">
         <v>50</v>
       </c>
       <c r="N47" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
     </row>
     <row r="48" spans="1:14">
@@ -3028,26 +3037,26 @@
       <c r="G48" t="s">
         <v>30</v>
       </c>
-      <c r="H48">
-        <v>1</v>
+      <c r="H48" t="s">
+        <v>17</v>
       </c>
       <c r="I48" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="J48">
         <v>67</v>
       </c>
       <c r="K48" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="L48" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="M48">
         <v>50</v>
       </c>
       <c r="N48" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
     </row>
     <row r="49" spans="1:14">
@@ -3072,26 +3081,26 @@
       <c r="G49" t="s">
         <v>31</v>
       </c>
-      <c r="H49">
-        <v>1</v>
+      <c r="H49" t="s">
+        <v>17</v>
       </c>
       <c r="I49" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="J49">
         <v>46</v>
       </c>
       <c r="K49" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="L49" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="M49">
         <v>50</v>
       </c>
       <c r="N49" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
     </row>
     <row r="50" spans="1:14">
@@ -3116,26 +3125,20 @@
       <c r="G50" t="s">
         <v>30</v>
       </c>
-      <c r="H50">
-        <v>1</v>
+      <c r="H50" t="s">
+        <v>32</v>
       </c>
       <c r="I50" t="s">
-        <v>56</v>
-      </c>
-      <c r="J50">
-        <v>50</v>
-      </c>
-      <c r="K50" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="L50" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="M50">
         <v>50</v>
       </c>
       <c r="N50" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
     </row>
     <row r="51" spans="1:14">
@@ -3160,26 +3163,26 @@
       <c r="G51" t="s">
         <v>30</v>
       </c>
-      <c r="H51">
-        <v>2</v>
+      <c r="H51" t="s">
+        <v>33</v>
       </c>
       <c r="I51" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="J51">
         <v>66</v>
       </c>
       <c r="K51" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="L51" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="M51">
         <v>50</v>
       </c>
       <c r="N51" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
     </row>
     <row r="52" spans="1:14">
@@ -3204,20 +3207,26 @@
       <c r="G52" t="s">
         <v>30</v>
       </c>
-      <c r="H52">
-        <v>3</v>
+      <c r="H52" t="s">
+        <v>34</v>
       </c>
       <c r="I52" t="s">
-        <v>58</v>
+        <v>61</v>
+      </c>
+      <c r="J52">
+        <v>50</v>
+      </c>
+      <c r="K52" t="s">
+        <v>78</v>
       </c>
       <c r="L52" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="M52">
         <v>50</v>
       </c>
       <c r="N52" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
     </row>
     <row r="53" spans="1:14">
@@ -3242,26 +3251,20 @@
       <c r="G53" t="s">
         <v>31</v>
       </c>
-      <c r="H53">
-        <v>1</v>
+      <c r="H53" t="s">
+        <v>32</v>
       </c>
       <c r="I53" t="s">
-        <v>56</v>
-      </c>
-      <c r="J53">
-        <v>47</v>
-      </c>
-      <c r="K53" t="s">
-        <v>76</v>
+        <v>59</v>
       </c>
       <c r="L53" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="M53">
         <v>50</v>
       </c>
       <c r="N53" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
     </row>
     <row r="54" spans="1:14">
@@ -3286,26 +3289,26 @@
       <c r="G54" t="s">
         <v>31</v>
       </c>
-      <c r="H54">
-        <v>2</v>
+      <c r="H54" t="s">
+        <v>33</v>
       </c>
       <c r="I54" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="J54">
         <v>47</v>
       </c>
       <c r="K54" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="L54" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="M54">
         <v>50</v>
       </c>
       <c r="N54" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
     </row>
     <row r="55" spans="1:14">
@@ -3330,20 +3333,26 @@
       <c r="G55" t="s">
         <v>31</v>
       </c>
-      <c r="H55">
-        <v>3</v>
+      <c r="H55" t="s">
+        <v>34</v>
       </c>
       <c r="I55" t="s">
-        <v>58</v>
+        <v>61</v>
+      </c>
+      <c r="J55">
+        <v>47</v>
+      </c>
+      <c r="K55" t="s">
+        <v>80</v>
       </c>
       <c r="L55" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="M55">
         <v>50</v>
       </c>
       <c r="N55" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
     </row>
     <row r="56" spans="1:14">
@@ -3368,26 +3377,20 @@
       <c r="G56" t="s">
         <v>30</v>
       </c>
-      <c r="H56">
-        <v>1</v>
+      <c r="H56" t="s">
+        <v>32</v>
       </c>
       <c r="I56" t="s">
-        <v>59</v>
-      </c>
-      <c r="J56">
-        <v>50</v>
-      </c>
-      <c r="K56" t="s">
-        <v>78</v>
+        <v>62</v>
       </c>
       <c r="L56" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="M56">
         <v>50</v>
       </c>
       <c r="N56" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
     </row>
     <row r="57" spans="1:14">
@@ -3412,26 +3415,26 @@
       <c r="G57" t="s">
         <v>30</v>
       </c>
-      <c r="H57">
-        <v>2</v>
+      <c r="H57" t="s">
+        <v>33</v>
       </c>
       <c r="I57" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="J57">
         <v>66</v>
       </c>
       <c r="K57" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="L57" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="M57">
         <v>50</v>
       </c>
       <c r="N57" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
     </row>
     <row r="58" spans="1:14">
@@ -3456,20 +3459,26 @@
       <c r="G58" t="s">
         <v>30</v>
       </c>
-      <c r="H58">
-        <v>3</v>
+      <c r="H58" t="s">
+        <v>34</v>
       </c>
       <c r="I58" t="s">
-        <v>61</v>
+        <v>64</v>
+      </c>
+      <c r="J58">
+        <v>50</v>
+      </c>
+      <c r="K58" t="s">
+        <v>82</v>
       </c>
       <c r="L58" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="M58">
         <v>50</v>
       </c>
       <c r="N58" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
     </row>
     <row r="59" spans="1:14">
@@ -3494,26 +3503,20 @@
       <c r="G59" t="s">
         <v>31</v>
       </c>
-      <c r="H59">
-        <v>1</v>
+      <c r="H59" t="s">
+        <v>32</v>
       </c>
       <c r="I59" t="s">
-        <v>59</v>
-      </c>
-      <c r="J59">
-        <v>47</v>
-      </c>
-      <c r="K59" t="s">
-        <v>80</v>
+        <v>62</v>
       </c>
       <c r="L59" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="M59">
         <v>50</v>
       </c>
       <c r="N59" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
     </row>
     <row r="60" spans="1:14">
@@ -3538,26 +3541,26 @@
       <c r="G60" t="s">
         <v>31</v>
       </c>
-      <c r="H60">
-        <v>2</v>
+      <c r="H60" t="s">
+        <v>33</v>
       </c>
       <c r="I60" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="J60">
         <v>47</v>
       </c>
       <c r="K60" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="L60" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="M60">
         <v>50</v>
       </c>
       <c r="N60" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
     </row>
     <row r="61" spans="1:14">
@@ -3582,20 +3585,26 @@
       <c r="G61" t="s">
         <v>31</v>
       </c>
-      <c r="H61">
-        <v>3</v>
+      <c r="H61" t="s">
+        <v>34</v>
       </c>
       <c r="I61" t="s">
-        <v>61</v>
+        <v>64</v>
+      </c>
+      <c r="J61">
+        <v>47</v>
+      </c>
+      <c r="K61" t="s">
+        <v>84</v>
       </c>
       <c r="L61" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="M61">
         <v>50</v>
       </c>
       <c r="N61" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
     </row>
   </sheetData>

</xml_diff>